<commit_message>
fix matrix tail row bug
</commit_message>
<xml_diff>
--- a/src/main/resources/SH600570.xlsx
+++ b/src/main/resources/SH600570.xlsx
@@ -2154,11 +2154,31 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>20210115</t>
+          <t>20210127</t>
         </is>
       </c>
       <c r="B210" t="n">
-        <v>9363.0</v>
+        <v>9260.0</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>20210218</t>
+        </is>
+      </c>
+      <c r="B211" t="n">
+        <v>10990.0</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>20210325</t>
+        </is>
+      </c>
+      <c r="B212" t="n">
+        <v>8013.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add matrix bspoint computer
</commit_message>
<xml_diff>
--- a/src/main/resources/SH600570.xlsx
+++ b/src/main/resources/SH600570.xlsx
@@ -2041,156 +2041,6 @@
         <v>7198.0</v>
       </c>
     </row>
-    <row r="199">
-      <c r="A199" t="inlineStr">
-        <is>
-          <t>20200709</t>
-        </is>
-      </c>
-      <c r="B199" t="n">
-        <v>12240.0</v>
-      </c>
-    </row>
-    <row r="200">
-      <c r="A200" t="inlineStr">
-        <is>
-          <t>20200812</t>
-        </is>
-      </c>
-      <c r="B200" t="n">
-        <v>9650.0</v>
-      </c>
-    </row>
-    <row r="201">
-      <c r="A201" t="inlineStr">
-        <is>
-          <t>20200831</t>
-        </is>
-      </c>
-      <c r="B201" t="n">
-        <v>11500.0</v>
-      </c>
-    </row>
-    <row r="202">
-      <c r="A202" t="inlineStr">
-        <is>
-          <t>20200917</t>
-        </is>
-      </c>
-      <c r="B202" t="n">
-        <v>9195.0</v>
-      </c>
-    </row>
-    <row r="203">
-      <c r="A203" t="inlineStr">
-        <is>
-          <t>20201013</t>
-        </is>
-      </c>
-      <c r="B203" t="n">
-        <v>10499.0</v>
-      </c>
-    </row>
-    <row r="204">
-      <c r="A204" t="inlineStr">
-        <is>
-          <t>20201102</t>
-        </is>
-      </c>
-      <c r="B204" t="n">
-        <v>8528.0</v>
-      </c>
-    </row>
-    <row r="205">
-      <c r="A205" t="inlineStr">
-        <is>
-          <t>20201110</t>
-        </is>
-      </c>
-      <c r="B205" t="n">
-        <v>9586.0</v>
-      </c>
-    </row>
-    <row r="206">
-      <c r="A206" t="inlineStr">
-        <is>
-          <t>20201126</t>
-        </is>
-      </c>
-      <c r="B206" t="n">
-        <v>8349.0</v>
-      </c>
-    </row>
-    <row r="207">
-      <c r="A207" t="inlineStr">
-        <is>
-          <t>20201209</t>
-        </is>
-      </c>
-      <c r="B207" t="n">
-        <v>10553.0</v>
-      </c>
-    </row>
-    <row r="208">
-      <c r="A208" t="inlineStr">
-        <is>
-          <t>20201225</t>
-        </is>
-      </c>
-      <c r="B208" t="n">
-        <v>9103.0</v>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" t="inlineStr">
-        <is>
-          <t>20210105</t>
-        </is>
-      </c>
-      <c r="B209" t="n">
-        <v>11059.0</v>
-      </c>
-    </row>
-    <row r="210">
-      <c r="A210" t="inlineStr">
-        <is>
-          <t>20210127</t>
-        </is>
-      </c>
-      <c r="B210" t="n">
-        <v>9260.0</v>
-      </c>
-    </row>
-    <row r="211">
-      <c r="A211" t="inlineStr">
-        <is>
-          <t>20210218</t>
-        </is>
-      </c>
-      <c r="B211" t="n">
-        <v>10990.0</v>
-      </c>
-    </row>
-    <row r="212">
-      <c r="A212" t="inlineStr">
-        <is>
-          <t>20210325</t>
-        </is>
-      </c>
-      <c r="B212" t="n">
-        <v>8013.0</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" t="inlineStr">
-        <is>
-          <t>20210406</t>
-        </is>
-      </c>
-      <c r="B213" t="n">
-        <v>8622.0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>